<commit_message>
access control overidable in custom project, adding template model
</commit_message>
<xml_diff>
--- a/hu.blackbelt.judo.generator.transformer.psm/src/model/PIM2PSM.xlsx
+++ b/hu.blackbelt.judo.generator.transformer.psm/src/model/PIM2PSM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="32">
   <si>
     <t xml:space="preserve">PIM</t>
   </si>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Gramm</t>
   </si>
   <si>
-    <t xml:space="preserve">Millimeter</t>
+    <t xml:space="preserve">Centimeter</t>
   </si>
   <si>
     <t xml:space="preserve">Forint</t>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">Szazalek</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IpCimMaszk</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
   <dimension ref="A1:B64"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+      <selection pane="topLeft" activeCell="K18" activeCellId="0" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -538,7 +541,7 @@
         <v>27</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,6 +566,14 @@
       </c>
       <c r="B29" s="0" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>